<commit_message>
separated emal function from main added logger webdriver options id passwor in env file
</commit_message>
<xml_diff>
--- a/Data/DateCheck.xlsx
+++ b/Data/DateCheck.xlsx
@@ -730,13 +730,13 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Q4</t>
+          <t>3Q2024</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>FY24 Half Year</t>
+          <t>FY25 Half Year</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>FetchingError</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">

</xml_diff>